<commit_message>
managed to create a read and write environment, sadly you need to change the filepath first for it to works in build environment
</commit_message>
<xml_diff>
--- a/Template_Database.xlsx
+++ b/Template_Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naiborab\Desktop\BootStapWithElectron\Door-Prize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431A0748-228E-4FE6-AB42-D6D7C1FFBED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01FF1F3-C821-4B33-95A2-CB53E8E7D479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FC90F8DD-72DA-4ADA-B9BF-1913B5EAB365}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>I00006</t>
+  </si>
+  <si>
+    <t>ISSELECTED</t>
+  </si>
+  <si>
+    <t>DOORPRICENAME</t>
   </si>
 </sst>
 </file>
@@ -167,12 +173,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D0A149B0-AECA-4965-8CA6-1D96444E3A62}" name="Table1" displayName="Table1" ref="A1:C11" totalsRowShown="0">
-  <autoFilter ref="A1:C11" xr:uid="{D0A149B0-AECA-4965-8CA6-1D96444E3A62}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D0A149B0-AECA-4965-8CA6-1D96444E3A62}" name="Table1" displayName="Table1" ref="A1:E11" totalsRowShown="0">
+  <autoFilter ref="A1:E11" xr:uid="{D0A149B0-AECA-4965-8CA6-1D96444E3A62}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{CB8157CD-4F55-45B7-86F4-ADF97B019DBB}" name="Name"/>
     <tableColumn id="2" xr3:uid="{F172052A-18DD-4E09-BE3D-DAB1A7E38E89}" name="KPK"/>
     <tableColumn id="3" xr3:uid="{1A6C7B40-9FBA-4D33-8D6B-D8DDF4A8411A}" name="Telephone Number"/>
+    <tableColumn id="4" xr3:uid="{328D40C1-17F2-42BC-90A4-A6A73F3C82E7}" name="ISSELECTED"/>
+    <tableColumn id="5" xr3:uid="{7454C194-5B04-46CB-AB43-448BAFF1AC26}" name="DOORPRICENAME"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -495,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89FCC88-3349-4F8B-9036-B44E215692A4}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,7 +516,7 @@
     <col min="3" max="3" width="18.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -518,8 +526,14 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -530,7 +544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -541,7 +555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -552,7 +566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -563,7 +577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -574,7 +588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -585,7 +599,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -596,7 +610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -607,7 +621,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -618,7 +632,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>

</xml_diff>